<commit_message>
base for the collab
</commit_message>
<xml_diff>
--- a/backend/public/temp/Work.xlsx
+++ b/backend/public/temp/Work.xlsx
@@ -5,27 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/FAAFE29EB3BFCFE5/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A933CED-B99B-48B7-BF08-F7774002656F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{37EC372B-06F4-4907-ABE7-9DE332A822F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2133FAB-EB26-486D-84E5-C47BBB2C0B62}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{497F3F51-FF14-476B-83BD-6523A818F5E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="164">
   <si>
     <t>User Name</t>
   </si>
@@ -33,487 +44,490 @@
     <t>Anushka Mishra</t>
   </si>
   <si>
+    <t>Vishesh</t>
+  </si>
+  <si>
     <t>Tejendra pratap singh</t>
   </si>
   <si>
+    <t>Aakash</t>
+  </si>
+  <si>
+    <t>Rajpurohit Yogesh kumar</t>
+  </si>
+  <si>
+    <t>Akshat Singh</t>
+  </si>
+  <si>
+    <t>Shivam Gupta</t>
+  </si>
+  <si>
+    <t>Aryan Kushwaha</t>
+  </si>
+  <si>
+    <t>Shilank jain</t>
+  </si>
+  <si>
+    <t>Vansh Jain</t>
+  </si>
+  <si>
+    <t>Rahul Bagdi</t>
+  </si>
+  <si>
+    <t>Neha Chaudhary</t>
+  </si>
+  <si>
+    <t>Nain Singh Rathore</t>
+  </si>
+  <si>
+    <t>Aarav Jain</t>
+  </si>
+  <si>
+    <t>Samman Gupta</t>
+  </si>
+  <si>
+    <t>Suthar Nidhi Upendrakumar</t>
+  </si>
+  <si>
+    <t>Yashsvi Garg</t>
+  </si>
+  <si>
+    <t>Sanket Jagdankar</t>
+  </si>
+  <si>
+    <t>Virag Jain</t>
+  </si>
+  <si>
+    <t>Anshuman</t>
+  </si>
+  <si>
+    <t>Prashant Kumar Gupta</t>
+  </si>
+  <si>
+    <t>Yatharth rohida</t>
+  </si>
+  <si>
+    <t>NISHA SONI</t>
+  </si>
+  <si>
+    <t>Akshat Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anshuman </t>
+  </si>
+  <si>
+    <t>Manish Upadhyay</t>
+  </si>
+  <si>
+    <t>Hardik Gupta</t>
+  </si>
+  <si>
+    <t>Suhani Yadav</t>
+  </si>
+  <si>
+    <t>Pratibha Khatri</t>
+  </si>
+  <si>
+    <t>NEHAL JAIN</t>
+  </si>
+  <si>
+    <t>Kunal Kushwaha</t>
+  </si>
+  <si>
+    <t>Priyanshu Malik</t>
+  </si>
+  <si>
+    <t>Rudraksh Puri</t>
+  </si>
+  <si>
+    <t>Shubhika Suraiya</t>
+  </si>
+  <si>
+    <t>Chirag Jain</t>
+  </si>
+  <si>
+    <t>Umang Bhardwaj</t>
+  </si>
+  <si>
+    <t>Deepesh Verma</t>
+  </si>
+  <si>
+    <t>Arjun</t>
+  </si>
+  <si>
+    <t>Divyanshi jain</t>
+  </si>
+  <si>
+    <t>AMISHKA SRIVASTAVA</t>
+  </si>
+  <si>
+    <t>Dhairya Maru</t>
+  </si>
+  <si>
+    <t>Navpreet Kaur</t>
+  </si>
+  <si>
+    <t>Sidharth Kumar</t>
+  </si>
+  <si>
+    <t>MAHIMA AGRAWAL</t>
+  </si>
+  <si>
+    <t>Uday Singh</t>
+  </si>
+  <si>
+    <t>Prasoon Sharma</t>
+  </si>
+  <si>
+    <t>Prachi Gupta</t>
+  </si>
+  <si>
+    <t>Ayush Porwal</t>
+  </si>
+  <si>
+    <t>Shiv Gupta</t>
+  </si>
+  <si>
+    <t>Harshit Dalve</t>
+  </si>
+  <si>
+    <t>Divyankar Raj</t>
+  </si>
+  <si>
+    <t>Girish Chandgothia</t>
+  </si>
+  <si>
+    <t>Ayush</t>
+  </si>
+  <si>
+    <t>Mahim kumar jain</t>
+  </si>
+  <si>
+    <t>Ketan Paliwal</t>
+  </si>
+  <si>
+    <t>Rituraj Sharma</t>
+  </si>
+  <si>
+    <t>Aryan Laxkar</t>
+  </si>
+  <si>
+    <t>Neeraj Meena</t>
+  </si>
+  <si>
+    <t>Shouryavardhan Singh</t>
+  </si>
+  <si>
+    <t>Aditya Agrawal</t>
+  </si>
+  <si>
+    <t>Rudra Pratap Singh</t>
+  </si>
+  <si>
+    <t>Shivam Rawtani</t>
+  </si>
+  <si>
+    <t>Anshika Bisht</t>
+  </si>
+  <si>
+    <t>Amit ahirwar</t>
+  </si>
+  <si>
+    <t>Rudra Pratap singh</t>
+  </si>
+  <si>
+    <t>Deepanshu Lath</t>
+  </si>
+  <si>
+    <t>Rajveer Singh Raghuvanshi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayush </t>
+  </si>
+  <si>
+    <t>Keshav Aggarwal</t>
+  </si>
+  <si>
+    <t>Dhiraj</t>
+  </si>
+  <si>
+    <t>Pranjal Swami</t>
+  </si>
+  <si>
+    <t>Manas kumar</t>
+  </si>
+  <si>
+    <t>Aryan</t>
+  </si>
+  <si>
+    <t>Raj Singhal</t>
+  </si>
+  <si>
+    <t>Dhanishka Sharma</t>
+  </si>
+  <si>
+    <t>Atharva Khokale</t>
+  </si>
+  <si>
+    <t>Jitesh Jhamnani</t>
+  </si>
+  <si>
+    <t>Aditya sharma</t>
+  </si>
+  <si>
+    <t>Jinansh Jain</t>
+  </si>
+  <si>
+    <t>Vansh Vats</t>
+  </si>
+  <si>
+    <t>Manan varyani</t>
+  </si>
+  <si>
+    <t>AYUSH YADAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhiraj </t>
+  </si>
+  <si>
+    <t>Devraj Prajapat</t>
+  </si>
+  <si>
+    <t>Divyanshi</t>
+  </si>
+  <si>
+    <t>Deepanshu Chauhan</t>
+  </si>
+  <si>
+    <t>Bhawna Chaudhary</t>
+  </si>
+  <si>
+    <t>saloni verma</t>
+  </si>
+  <si>
+    <t>Vaishali Gupta</t>
+  </si>
+  <si>
+    <t>Shreya Hole</t>
+  </si>
+  <si>
+    <t>Sweta Jaiswal</t>
+  </si>
+  <si>
+    <t>Bhoomika Bhatia</t>
+  </si>
+  <si>
+    <t>Avighna Tripathi</t>
+  </si>
+  <si>
+    <t>Aashil Singhal</t>
+  </si>
+  <si>
+    <t>Mohd Asheer</t>
+  </si>
+  <si>
+    <t>Nishika Roy</t>
+  </si>
+  <si>
+    <t>Bharti Dhote</t>
+  </si>
+  <si>
+    <t>Arman</t>
+  </si>
+  <si>
+    <t>Ankit Swami</t>
+  </si>
+  <si>
+    <t>Kasshan Khan</t>
+  </si>
+  <si>
+    <t>Om</t>
+  </si>
+  <si>
+    <t>Tanveer Singh</t>
+  </si>
+  <si>
+    <t>Lakshya Sharma</t>
+  </si>
+  <si>
+    <t>Kashish Bhutia</t>
+  </si>
+  <si>
+    <t>Shikhar Asthana</t>
+  </si>
+  <si>
+    <t>AMBIKA SHARMA</t>
+  </si>
+  <si>
+    <t>Aayush Vijay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aryan </t>
+  </si>
+  <si>
+    <t>Shreyansh Jaiswal</t>
+  </si>
+  <si>
+    <t>Sumit goyal</t>
+  </si>
+  <si>
+    <t>Advik Saksena</t>
+  </si>
+  <si>
+    <t>Amitesh Gupta</t>
+  </si>
+  <si>
+    <t>Pearl Jain</t>
+  </si>
+  <si>
+    <t>Jayant Kothari</t>
+  </si>
+  <si>
+    <t>Aakarsh Bibhaw</t>
+  </si>
+  <si>
+    <t>Raghvendra Singh</t>
+  </si>
+  <si>
+    <t>om</t>
+  </si>
+  <si>
     <t>Chaudhary Nutankumari Sanjaykumar</t>
   </si>
   <si>
+    <t>Parvika</t>
+  </si>
+  <si>
     <t>Himani goel</t>
   </si>
   <si>
-    <t>Akshat Sharma</t>
+    <t>Divyansha Yadav</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t>Pragya Shree</t>
+  </si>
+  <si>
+    <t>Apoorva Shree</t>
+  </si>
+  <si>
+    <t>Anubha Priyanka Toppo</t>
+  </si>
+  <si>
+    <t>Diya Taneja</t>
+  </si>
+  <si>
+    <t>Chavi Bansal</t>
+  </si>
+  <si>
+    <t>Neha singh</t>
+  </si>
+  <si>
+    <t>Sidhi Jha</t>
+  </si>
+  <si>
+    <t>Min Jiya Vinaybhai</t>
+  </si>
+  <si>
+    <t>Lovelish</t>
+  </si>
+  <si>
+    <t>Akshita Singh</t>
+  </si>
+  <si>
+    <t>Sanika Sharma</t>
   </si>
   <si>
     <t>Keshav Tambi</t>
   </si>
   <si>
-    <t>Ayush Porwal</t>
-  </si>
-  <si>
-    <t>Samman Gupta</t>
-  </si>
-  <si>
-    <t>Divyansha Yadav</t>
+    <t xml:space="preserve">Siddhant </t>
   </si>
   <si>
     <t>Burhanuddin Kankroli Wala</t>
   </si>
   <si>
-    <t>Manish Upadhyay</t>
-  </si>
-  <si>
-    <t>Jasmine</t>
-  </si>
-  <si>
-    <t>Girish Chandgothia</t>
-  </si>
-  <si>
-    <t>Hardik Gupta</t>
-  </si>
-  <si>
-    <t>Rajpurohit Yogesh kumar</t>
-  </si>
-  <si>
-    <t>Akshat Singh</t>
+    <t>Kishlay Yashvardhan</t>
+  </si>
+  <si>
+    <t>SHELLY CHARAS</t>
+  </si>
+  <si>
+    <t>Akshay Rawat</t>
+  </si>
+  <si>
+    <t>Shivang Singh</t>
+  </si>
+  <si>
+    <t>Suyash Suiwala</t>
+  </si>
+  <si>
+    <t>Happy Mandowara</t>
+  </si>
+  <si>
+    <t>Shrine Singh</t>
+  </si>
+  <si>
+    <t>Tulsi meena</t>
+  </si>
+  <si>
+    <t>Shashank Gupta</t>
+  </si>
+  <si>
+    <t>Harsh Popat</t>
+  </si>
+  <si>
+    <t>Prakhar Mahaur</t>
+  </si>
+  <si>
+    <t>Shivansh Dwivedi</t>
+  </si>
+  <si>
+    <t>Tanmay sharma</t>
   </si>
   <si>
     <t>Tanmay Saxena</t>
   </si>
   <si>
-    <t>Shikhar Asthana</t>
-  </si>
-  <si>
-    <t>AMBIKA SHARMA</t>
-  </si>
-  <si>
     <t>Mohd Farhan Ahmad</t>
   </si>
   <si>
-    <t>Kishlay Yashvardhan</t>
-  </si>
-  <si>
-    <t>Aayush Vijay</t>
-  </si>
-  <si>
-    <t>Pragya Shree</t>
-  </si>
-  <si>
-    <t>SHELLY CHARAS</t>
-  </si>
-  <si>
-    <t>Keshav Aggarwal</t>
-  </si>
-  <si>
-    <t>Mahim kumar jain</t>
-  </si>
-  <si>
-    <t>Devraj Prajapat</t>
-  </si>
-  <si>
-    <t>Shivam Gupta</t>
-  </si>
-  <si>
-    <t>Apoorva Shree</t>
-  </si>
-  <si>
-    <t>Ketan Paliwal</t>
-  </si>
-  <si>
-    <t>Rituraj Sharma</t>
-  </si>
-  <si>
-    <t>Deepanshu Chauhan</t>
-  </si>
-  <si>
-    <t>Akshay Rawat</t>
-  </si>
-  <si>
-    <t>Aryan Kushwaha</t>
-  </si>
-  <si>
-    <t>Aryan Laxkar</t>
-  </si>
-  <si>
-    <t>NISHA SONI</t>
-  </si>
-  <si>
-    <t>Bhawna Chaudhary</t>
-  </si>
-  <si>
-    <t>Neeraj Meena</t>
-  </si>
-  <si>
     <t>Parth Bhardwaj</t>
   </si>
   <si>
-    <t>Suhani Yadav</t>
-  </si>
-  <si>
-    <t>Shouryavardhan Singh</t>
-  </si>
-  <si>
-    <t>Anubha Priyanka Toppo</t>
-  </si>
-  <si>
-    <t>Shiv Gupta</t>
-  </si>
-  <si>
-    <t>saloni verma</t>
-  </si>
-  <si>
-    <t>Vaishali Gupta</t>
-  </si>
-  <si>
-    <t>Shivang Singh</t>
-  </si>
-  <si>
     <t>Arpit Sharma</t>
   </si>
   <si>
-    <t>Suthar Nidhi Upendrakumar</t>
-  </si>
-  <si>
-    <t>Pratibha Khatri</t>
-  </si>
-  <si>
-    <t>Shreya Hole</t>
-  </si>
-  <si>
     <t>Shreyas Gurjar</t>
   </si>
   <si>
-    <t>NEHAL JAIN</t>
-  </si>
-  <si>
-    <t>Diya Taneja</t>
-  </si>
-  <si>
-    <t>Suyash Suiwala</t>
-  </si>
-  <si>
-    <t>Kunal Kushwaha</t>
-  </si>
-  <si>
-    <t>Sweta Jaiswal</t>
-  </si>
-  <si>
-    <t>Aditya Agrawal</t>
-  </si>
-  <si>
-    <t>Yashsvi Garg</t>
-  </si>
-  <si>
-    <t>Divyanshi jain</t>
-  </si>
-  <si>
-    <t>Pranjal Swami</t>
-  </si>
-  <si>
-    <t>Tanveer Singh</t>
-  </si>
-  <si>
     <t>Utkarsh likhar</t>
   </si>
   <si>
-    <t>Manas kumar</t>
-  </si>
-  <si>
-    <t>Aryan</t>
-  </si>
-  <si>
-    <t>Rudra Pratap Singh</t>
-  </si>
-  <si>
     <t>Ayush Pratap Singh</t>
   </si>
   <si>
-    <t>Deepesh Verma</t>
-  </si>
-  <si>
-    <t>AYUSH YADAV</t>
-  </si>
-  <si>
-    <t>AMISHKA SRIVASTAVA</t>
-  </si>
-  <si>
-    <t>Shivam Rawtani</t>
-  </si>
-  <si>
-    <t>Dhairya Maru</t>
-  </si>
-  <si>
-    <t>Shreyansh Jaiswal</t>
-  </si>
-  <si>
-    <t>Navpreet Kaur</t>
-  </si>
-  <si>
-    <t>Bhoomika Bhatia</t>
-  </si>
-  <si>
     <t>Aman Yadav</t>
   </si>
   <si>
-    <t>Raj Singhal</t>
-  </si>
-  <si>
-    <t>Avighna Tripathi</t>
-  </si>
-  <si>
     <t>Rishi Agarwal</t>
   </si>
   <si>
-    <t>Dhanishka Sharma</t>
-  </si>
-  <si>
-    <t>Sidharth Kumar</t>
-  </si>
-  <si>
-    <t>MAHIMA AGRAWAL</t>
-  </si>
-  <si>
-    <t>Aashil Singhal</t>
-  </si>
-  <si>
-    <t>Atharva Khokale</t>
-  </si>
-  <si>
-    <t>Priyanshu Malik</t>
-  </si>
-  <si>
-    <t>Harshit Dalve</t>
-  </si>
-  <si>
-    <t>Jitesh Jhamnani</t>
-  </si>
-  <si>
-    <t>Mohd Asheer</t>
-  </si>
-  <si>
-    <t>Nishika Roy</t>
-  </si>
-  <si>
-    <t>Bharti Dhote</t>
-  </si>
-  <si>
-    <t>Anshika Bisht</t>
-  </si>
-  <si>
-    <t>Sumit goyal</t>
-  </si>
-  <si>
-    <t>Uday Singh</t>
-  </si>
-  <si>
-    <t>Advik Saksena</t>
-  </si>
-  <si>
-    <t>Rudraksh Puri</t>
-  </si>
-  <si>
-    <t>Amitesh Gupta</t>
-  </si>
-  <si>
-    <t>Chavi Bansal</t>
-  </si>
-  <si>
-    <t>Pearl Jain</t>
-  </si>
-  <si>
-    <t>Jayant Kothari</t>
-  </si>
-  <si>
-    <t>Shubhika Suraiya</t>
-  </si>
-  <si>
     <t>Abhishek singh parmar</t>
   </si>
   <si>
     <t>Sahil kumar</t>
   </si>
   <si>
-    <t>Divyankar Raj</t>
-  </si>
-  <si>
-    <t>Lakshya Sharma</t>
-  </si>
-  <si>
-    <t>Virag Jain</t>
-  </si>
-  <si>
-    <t>Arman</t>
-  </si>
-  <si>
-    <t>Neha singh</t>
-  </si>
-  <si>
-    <t>Sidhi Jha</t>
-  </si>
-  <si>
-    <t>Shilank jain</t>
-  </si>
-  <si>
-    <t>Ankit Swami</t>
-  </si>
-  <si>
-    <t>Prashant Kumar Gupta</t>
-  </si>
-  <si>
-    <t>Happy Mandowara</t>
-  </si>
-  <si>
-    <t>Vansh Jain</t>
-  </si>
-  <si>
-    <t>Chirag Jain</t>
-  </si>
-  <si>
-    <t>Min Jiya Vinaybhai</t>
-  </si>
-  <si>
-    <t>Lovelish</t>
-  </si>
-  <si>
-    <t>Aditya sharma</t>
-  </si>
-  <si>
-    <t>Jinansh Jain</t>
-  </si>
-  <si>
-    <t>Kasshan Khan</t>
-  </si>
-  <si>
-    <t>Shrine Singh</t>
-  </si>
-  <si>
-    <t>Rahul Bagdi</t>
-  </si>
-  <si>
-    <t>Aakarsh Bibhaw</t>
-  </si>
-  <si>
-    <t>Tulsi meena</t>
-  </si>
-  <si>
     <t>Priyanshu Arora</t>
   </si>
   <si>
-    <t>Akshita Singh</t>
-  </si>
-  <si>
-    <t>Tanmay sharma</t>
-  </si>
-  <si>
-    <t>Amit ahirwar</t>
-  </si>
-  <si>
     <t>ADITYA KUMAR</t>
   </si>
   <si>
-    <t>Vansh Vats</t>
-  </si>
-  <si>
-    <t>Neha Chaudhary</t>
-  </si>
-  <si>
-    <t>Nain Singh Rathore</t>
-  </si>
-  <si>
-    <t>Prasoon Sharma</t>
-  </si>
-  <si>
-    <t>Rudra Pratap singh</t>
-  </si>
-  <si>
-    <t>Umang Bhardwaj</t>
-  </si>
-  <si>
-    <t>Shashank Gupta</t>
-  </si>
-  <si>
-    <t>Deepanshu Lath</t>
-  </si>
-  <si>
-    <t>Aarav Jain</t>
-  </si>
-  <si>
     <t>Tarun Tiwari</t>
-  </si>
-  <si>
-    <t>Harsh Popat</t>
-  </si>
-  <si>
-    <t>Rajveer Singh Raghuvanshi</t>
-  </si>
-  <si>
-    <t>Raghvendra Singh</t>
-  </si>
-  <si>
-    <t>Yatharth rohida</t>
-  </si>
-  <si>
-    <t>Prakhar Mahaur</t>
-  </si>
-  <si>
-    <t>Shivansh Dwivedi</t>
-  </si>
-  <si>
-    <t>Sanika Sharma</t>
-  </si>
-  <si>
-    <t>Manan varyani</t>
-  </si>
-  <si>
-    <t>Sanket Jagdankar</t>
-  </si>
-  <si>
-    <t>Kashish Bhutia</t>
-  </si>
-  <si>
-    <t>Prachi Gupta</t>
-  </si>
-  <si>
-    <t>Vishesh</t>
-  </si>
-  <si>
-    <t>Aakash</t>
-  </si>
-  <si>
-    <t>Parvika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anshuman </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siddhant </t>
-  </si>
-  <si>
-    <t>Om</t>
-  </si>
-  <si>
-    <t>Ayush</t>
-  </si>
-  <si>
-    <t>Dhiraj</t>
-  </si>
-  <si>
-    <t>Divyanshi</t>
-  </si>
-  <si>
-    <t>Arjun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhiraj </t>
-  </si>
-  <si>
-    <t>Anshuman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ayush </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aryan </t>
   </si>
 </sst>
 </file>
@@ -900,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247B853A-790E-4465-A71A-B188F0E37486}">
   <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -922,1626 +936,1626 @@
         <v>2029</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2029</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>2029</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2029</v>
       </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>2029</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>2029</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>2029</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>2029</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>2028</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>129</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>2028</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>2028</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>136</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>2029</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16">
-        <v>2029</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5">
         <v>2029</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>2029</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>2029</v>
       </c>
       <c r="C20" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>2029</v>
       </c>
       <c r="C21" t="s">
-        <v>160</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>2029</v>
       </c>
       <c r="C22" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>2029</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>2029</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>2029</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>2029</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>2029</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>2029</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>2029</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>2029</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>2028</v>
       </c>
       <c r="C31" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>2029</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>133</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>2029</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>2029</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B35">
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B36">
         <v>2029</v>
       </c>
       <c r="C36" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="B37">
         <v>2028</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <v>2029</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <v>2029</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B40">
         <v>2029</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="B41">
         <v>2028</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="B42">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="B43">
         <v>2028</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>131</v>
+        <v>48</v>
       </c>
       <c r="B44">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="C44" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>146</v>
+        <v>49</v>
+      </c>
+      <c r="B45">
+        <v>2029</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="B46">
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B47">
-        <v>2028</v>
+        <v>51</v>
+      </c>
+      <c r="B47" s="4">
+        <v>2029</v>
       </c>
       <c r="C47" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B48">
         <v>2029</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B49">
         <v>2029</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>2029</v>
       </c>
       <c r="C50" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B51">
         <v>2029</v>
       </c>
       <c r="C51" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B52">
         <v>2029</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>2029</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>2029</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>2029</v>
       </c>
       <c r="C55" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>2029</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B57">
         <v>2029</v>
       </c>
       <c r="C57" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B58">
         <v>2028</v>
       </c>
       <c r="C58" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="B59">
         <v>2028</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="B60">
         <v>2029</v>
       </c>
       <c r="C60" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
       <c r="B61">
         <v>2029</v>
       </c>
       <c r="C61" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="B62">
         <v>2029</v>
       </c>
       <c r="C62" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="B63">
         <v>2029</v>
       </c>
       <c r="C63" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B64">
         <v>2029</v>
       </c>
       <c r="C64" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B65">
         <v>2029</v>
       </c>
       <c r="C65" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B66">
         <v>2029</v>
       </c>
       <c r="C66" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B67">
         <v>2027</v>
       </c>
       <c r="C67" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B68">
         <v>2027</v>
       </c>
       <c r="C68" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B69">
         <v>2027</v>
       </c>
       <c r="C69" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B70">
         <v>2027</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="B71">
         <v>2029</v>
       </c>
       <c r="C71" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="B72">
         <v>2028</v>
       </c>
       <c r="C72" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="B73">
         <v>2028</v>
       </c>
       <c r="C73" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B74">
         <v>2029</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B75">
         <v>2029</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="B76">
         <v>2027</v>
       </c>
       <c r="C76" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="B77">
         <v>2027</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B78">
         <v>2027</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B79">
         <v>2027</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B80">
         <v>2027</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B81">
         <v>2027</v>
       </c>
       <c r="C81" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B82">
         <v>2027</v>
       </c>
       <c r="C82" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B83">
         <v>2027</v>
       </c>
       <c r="C83" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B84">
         <v>2027</v>
       </c>
       <c r="C84" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B85">
         <v>2027</v>
       </c>
       <c r="C85" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B86">
         <v>2027</v>
       </c>
       <c r="C86" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B87">
         <v>2027</v>
       </c>
       <c r="C87" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B88">
         <v>2027</v>
       </c>
       <c r="C88" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B89">
         <v>2027</v>
       </c>
       <c r="C89" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B90">
         <v>2027</v>
       </c>
       <c r="C90" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="B91">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="C91" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="B92">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="C92" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="B93">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="C93" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="B94">
         <v>2027</v>
       </c>
       <c r="C94" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="B95">
         <v>2029</v>
       </c>
       <c r="C95" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A96" s="3" t="s">
-        <v>162</v>
+      <c r="A96" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="B96">
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="C96" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B97">
         <v>2027</v>
       </c>
       <c r="C97" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A98" s="1" t="s">
-        <v>85</v>
+      <c r="A98" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="B98">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="C98" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B99">
         <v>2027</v>
       </c>
       <c r="C99" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B100">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C100" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B101">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="C101" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B102">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="C102" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="B103">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="C103" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B104" s="4">
-        <v>2029</v>
+        <v>114</v>
+      </c>
+      <c r="B104">
+        <v>2027</v>
       </c>
       <c r="C104" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B105">
         <v>2028</v>
       </c>
       <c r="C105" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="B106">
         <v>2028</v>
       </c>
       <c r="C106" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="B107">
         <v>2029</v>
       </c>
       <c r="C107" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="B108">
         <v>2029</v>
       </c>
       <c r="C108" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="B109">
         <v>2029</v>
       </c>
       <c r="C109" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="B110">
         <v>2029</v>
       </c>
       <c r="C110" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="B111">
         <v>2029</v>
       </c>
       <c r="C111" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="B112">
         <v>2029</v>
       </c>
       <c r="C112" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="B113">
         <v>2029</v>
       </c>
       <c r="C113" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="B114">
         <v>2029</v>
       </c>
       <c r="C114" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="B115">
         <v>2029</v>
       </c>
       <c r="C115" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="B116">
         <v>2029</v>
       </c>
       <c r="C116" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="B117">
         <v>2029</v>
       </c>
       <c r="C117" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="B118">
         <v>2029</v>
       </c>
       <c r="C118" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B119">
         <v>2029</v>
       </c>
       <c r="C119" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B120">
         <v>2029</v>
       </c>
       <c r="C120" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B121">
         <v>2029</v>
       </c>
       <c r="C121" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="C122" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="B123">
         <v>2029</v>
       </c>
       <c r="C123" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
       <c r="B124">
         <v>2029</v>
       </c>
       <c r="C124" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="B125">
         <v>2029</v>
       </c>
       <c r="C125" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="B126">
         <v>2029</v>
       </c>
       <c r="C126" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="B127">
         <v>2029</v>
       </c>
       <c r="C127" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="B128">
         <v>2029</v>
       </c>
       <c r="C128" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" s="1" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="B129">
         <v>2029</v>
       </c>
       <c r="C129" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="B130">
         <v>2028</v>
       </c>
       <c r="C130" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="B131">
         <v>2029</v>
       </c>
       <c r="C131" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" s="1" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B132">
         <v>2028</v>
       </c>
       <c r="C132" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B133">
         <v>2029</v>
       </c>
       <c r="C133" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B134">
         <v>2028</v>
       </c>
       <c r="C134" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B135">
         <v>2029</v>
       </c>
       <c r="C135" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" s="1" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="B136">
         <v>2028</v>
       </c>
       <c r="C136" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" s="1" t="s">
-        <v>17</v>
+        <v>150</v>
       </c>
       <c r="B137">
         <v>2029</v>
       </c>
       <c r="C137" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" s="1" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="B138">
         <v>2029</v>
       </c>
       <c r="C138" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" s="1" t="s">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="B139">
         <v>2029</v>
       </c>
       <c r="C139" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" s="1" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="B140">
         <v>2029</v>
       </c>
       <c r="C140" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" s="1" t="s">
-        <v>51</v>
+        <v>154</v>
       </c>
       <c r="B141">
         <v>2029</v>
       </c>
       <c r="C141" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142" s="1" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="B142">
         <v>2029</v>
       </c>
       <c r="C142" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" s="1" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="B143">
         <v>2029</v>
       </c>
       <c r="C143" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" s="1" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
       <c r="B144">
         <v>2029</v>
       </c>
       <c r="C144" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" s="1" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="B145">
         <v>2029</v>
       </c>
       <c r="C145" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" s="1" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="B146">
         <v>2029</v>
       </c>
       <c r="C146" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" s="1" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="B147">
         <v>2027</v>
       </c>
       <c r="C147" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148" s="1" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="B148">
         <v>2028</v>
       </c>
       <c r="C148" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" s="1" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="B149">
         <v>2028</v>
       </c>
       <c r="C149" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" s="1" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="B150">
         <v>2029</v>
       </c>
       <c r="C150" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
@@ -2578,8 +2592,8 @@
       <c r="A161" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C161">
-    <sortCondition ref="C34:C161"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C150">
+    <sortCondition ref="C43:C150"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>